<commit_message>
regression validation + mcs probing inferences
</commit_message>
<xml_diff>
--- a/measurement_client_standalone/output/distance-based/CRUSP Distance-Based Measures.xlsx
+++ b/measurement_client_standalone/output/distance-based/CRUSP Distance-Based Measures.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinni\source\repos\Research\measurement_client_standalone\output\distance-based\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56418B75-1FA6-42CF-85A1-A87C25559561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04460BBE-EA67-4AFC-BC18-360C99D81027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{F5C78390-FA3F-4EED-A8F8-5CF0F36478F2}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
   <si>
     <t>downlink_2-6-23-base average bandwidth: 74.4531349 Mbps</t>
   </si>
@@ -123,6 +124,93 @@
   </si>
   <si>
     <t>Increase</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>validation:</t>
+  </si>
+  <si>
+    <t>downlink_rtest-1 average bandwidth: 45.68223942499999 Mbps</t>
+  </si>
+  <si>
+    <t>downlink_rtest-1 average packets received: 896.15/930</t>
+  </si>
+  <si>
+    <t>downlink_rtest-2 average bandwidth: 32.59307200000001 Mbps</t>
+  </si>
+  <si>
+    <t>downlink_rtest-2 average packets received: 913.25/930</t>
+  </si>
+  <si>
+    <t>downlink_rtest-3 average bandwidth: 39.054063600000006 Mbps</t>
+  </si>
+  <si>
+    <t>downlink_rtest-3 average packets received: 927.5/930</t>
+  </si>
+  <si>
+    <t>downlink_rtest-4 average bandwidth: 77.20655905000002 Mbps</t>
+  </si>
+  <si>
+    <t>downlink_rtest-4 average packets received: 920.3/930</t>
+  </si>
+  <si>
+    <t>uplink_rtest-1 average bandwidth: 27.871669500000007 Mbps</t>
+  </si>
+  <si>
+    <t>uplink_rtest-1 average packets received: 361.3/930</t>
+  </si>
+  <si>
+    <t>uplink_rtest-2 average bandwidth: 25.06290505 Mbps</t>
+  </si>
+  <si>
+    <t>uplink_rtest-2 average packets received: 324.65/930</t>
+  </si>
+  <si>
+    <t>uplink_rtest-3 average bandwidth: 20.00212342 Mbps</t>
+  </si>
+  <si>
+    <t>uplink_rtest-3 average packets received: 209.45/930</t>
+  </si>
+  <si>
+    <t>uplink_rtest-4 average bandwidth: 31.97023575 Mbps</t>
+  </si>
+  <si>
+    <t>uplink_rtest-4 average packets received: 419.0/930</t>
+  </si>
+  <si>
+    <t>CRUSP
+ Uplink</t>
+  </si>
+  <si>
+    <t>Iperf3 Sender 
+(Ground Truth)</t>
+  </si>
+  <si>
+    <t>Regression
+Predicted</t>
+  </si>
+  <si>
+    <t>% Difference</t>
+  </si>
+  <si>
+    <t>MAPE (Mean Absolute Percentage Error)</t>
+  </si>
+  <si>
+    <t>Ground Truth</t>
+  </si>
+  <si>
+    <t>rtest1</t>
+  </si>
+  <si>
+    <t>rtest2</t>
+  </si>
+  <si>
+    <t>rtest3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transmit rate (Mbps)   </t>
   </si>
 </sst>
 </file>
@@ -368,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -403,9 +491,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -415,7 +500,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -436,11 +521,74 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="22">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -465,20 +613,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2776,7 +2910,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:trendline>
             <c:spPr>
@@ -3247,13 +3393,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Iperf3</a:t>
+              <a:t>CRUSP Uplink vs Iperf3</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs. CRUSP Uplink</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3982,6 +4123,1384 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CRUSP Uplink vs Iperf3</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (Adjusted)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AO$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ground Truth</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AN$6:$AN$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>27.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60.584000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.827999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8849999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.476</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AO$6:$AO$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>17.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1500000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-14F3-45A6-82AA-4D4A1FE334FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="984335600"/>
+        <c:axId val="984333936"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="984335600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CRUSP Uplink (Mbps)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="984333936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="984333936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iperf3 (Mbps)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="984335600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>CRUSP Uplink vs Iperf3</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (Validation)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inside-LOS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>20.827999999999999</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>13.4</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4B33-4A49-A150-B22B5900A3CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Right-Outside</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>5.476</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>4.1500000000000004</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4B33-4A49-A150-B22B5900A3CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Baseline</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>60.584000000000003</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>43.7</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4B33-4A49-A150-B22B5900A3CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Inside-No-LOS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>5.8849999999999998</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>3.45</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4B33-4A49-A150-B22B5900A3CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Combined</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.15095330713781924"/>
+                  <c:y val="-4.0372400960460476E-4"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t>y = 0.7283x - 0.7162</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$13:$S$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60.584000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.827999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8849999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.476</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$12:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>43.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1500000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-4B33-4A49-A150-B22B5900A3CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>R-Tests</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>27.87</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>25.06</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>31.97</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="3"/>
+              <c:pt idx="0">
+                <c:v>17.2</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>16.8</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>32.700000000000003</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-4B33-4A49-A150-B22B5900A3CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1115645360"/>
+        <c:axId val="1115654512"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1115645360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>CRUSP Uplink (Mbps)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1115654512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1115654512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iperf3 Ground Truth (Mbps)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1115645360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="6"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="7"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4222,6 +5741,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6751,6 +8350,1038 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7378,16 +10009,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>611665</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>12246</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>263716</xdr:rowOff>
+      <xdr:rowOff>314547</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>281160</xdr:colOff>
+      <xdr:colOff>328081</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>17213</xdr:rowOff>
+      <xdr:rowOff>61266</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7486,25 +10117,99 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>132199</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>32517</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>163401</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66019</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D4041AE-517C-7496-E548-6BC082E90EC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>745101</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>161311</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>247335</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>80352</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FECDDA17-3556-4F1F-98FC-9B920D5E5F3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{153DAB2C-EF94-4E6C-ACF1-75466A92B359}" name="Table2" displayName="Table2" ref="I2:M6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{153DAB2C-EF94-4E6C-ACF1-75466A92B359}" name="Table2" displayName="Table2" ref="I2:M6" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="I2:M6" xr:uid="{153DAB2C-EF94-4E6C-ACF1-75466A92B359}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{41E00012-EF48-4186-8C46-FAC1FFE784AB}" name="Column1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{159C8C02-763A-4537-A836-8808E2FBE3B0}" name="Base" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{1650172B-D89B-425B-BF85-42BE021150A6}" name="Inside-LOS" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{3B346FA8-1702-4383-AE51-50F0E0BA6292}" name="Inside-No-LOS" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{DF38FAD1-CF60-420C-ADBC-C8EAF257A320}" name="Right-Outside" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{41E00012-EF48-4186-8C46-FAC1FFE784AB}" name="Column1" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{159C8C02-763A-4537-A836-8808E2FBE3B0}" name="Base" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{1650172B-D89B-425B-BF85-42BE021150A6}" name="Inside-LOS" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{3B346FA8-1702-4383-AE51-50F0E0BA6292}" name="Inside-No-LOS" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{DF38FAD1-CF60-420C-ADBC-C8EAF257A320}" name="Right-Outside" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8ED2F1E2-6AA3-42CE-861D-FBE0310EABCA}" name="Table1" displayName="Table1" ref="O11:S15" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8ED2F1E2-6AA3-42CE-861D-FBE0310EABCA}" name="Table1" displayName="Table1" ref="O11:S15" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="O11:S15" xr:uid="{8ED2F1E2-6AA3-42CE-861D-FBE0310EABCA}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DAC16C73-CF2C-4B33-AD03-E24ECF7E1E81}" name="Column1"/>
@@ -7514,6 +10219,44 @@
     <tableColumn id="5" xr3:uid="{4D042B30-DF80-47E2-8DC9-2C3E91BBFEB6}" name="Right-Outside"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{59F9924A-A968-4FC6-A4AF-E49BD1A5FACC}" name="Table5" displayName="Table5" ref="AD5:AG7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="AD5:AG7" xr:uid="{59F9924A-A968-4FC6-A4AF-E49BD1A5FACC}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{7799797F-C817-424E-BB5D-16D13AF256CF}" name="Column1" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{1B6ECD86-4CCE-4203-B798-EBE6080D819C}" name="rtest1" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{AF847395-FD25-4E73-828E-0622476D2FBE}" name="rtest2" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{690DD896-6776-4915-82D2-6AE74E19ABDE}" name="rtest3" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E1D211B0-884F-41F7-89EC-10D254236712}" name="Table6" displayName="Table6" ref="AD13:AG17" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="AD13:AG17" xr:uid="{E1D211B0-884F-41F7-89EC-10D254236712}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{4FFC0EA4-D6BB-45BF-A83F-98593EF47852}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{70AB4688-4286-4CF5-940F-E3BF42D4C693}" name="rtest1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{2E4CE3C5-1BD1-434E-96A0-2ECB4D4389BB}" name="rtest2" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{58B2890E-50B7-4A9F-80C3-0461572BC08C}" name="rtest3" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{EC923B3A-B5F0-4918-B4AA-41FF2C338186}" name="Table7" displayName="Table7" ref="AV4:AX14" totalsRowShown="0">
+  <autoFilter ref="AV4:AX14" xr:uid="{EC923B3A-B5F0-4918-B4AA-41FF2C338186}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{39967C65-F6DE-4496-B8BF-E5840F41518A}" name="rtest1"/>
+    <tableColumn id="2" xr3:uid="{74AA46B2-FD50-4D01-964B-3EF088A68C0F}" name="rtest2"/>
+    <tableColumn id="3" xr3:uid="{FB12E138-46BD-4E41-910E-B0BF6C64308F}" name="rtest3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -7814,10 +10557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CDA644-4291-4C70-B6C3-35B671A5F97E}">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:AX56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R24" zoomScale="93" workbookViewId="0">
-      <selection activeCell="AC41" sqref="AC41"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="58" workbookViewId="0">
+      <selection activeCell="AV4" sqref="AV4:AX14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7830,14 +10573,16 @@
     <col min="17" max="17" width="11.1328125" customWidth="1"/>
     <col min="18" max="18" width="14.19921875" customWidth="1"/>
     <col min="19" max="19" width="13.73046875" customWidth="1"/>
+    <col min="30" max="30" width="12.46484375" customWidth="1"/>
+    <col min="31" max="33" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:50" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -7857,7 +10602,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:50" ht="15" x14ac:dyDescent="0.45">
       <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
@@ -7874,7 +10619,7 @@
         <v>19.984000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:50" ht="30" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -7908,23 +10653,39 @@
       <c r="S4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="U4" s="20" t="s">
+      <c r="U4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="V4" s="21" t="s">
+      <c r="V4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="21" t="s">
+      <c r="W4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="X4" s="21" t="s">
+      <c r="X4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="Y4" s="22" t="s">
+      <c r="Y4" s="21" t="s">
         <v>19</v>
       </c>
+      <c r="AD4" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE4" s="22"/>
+      <c r="AF4" s="22"/>
+      <c r="AG4" s="22"/>
+      <c r="AH4" s="22"/>
+      <c r="AV4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="5" spans="1:25" ht="60" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:50" ht="60" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -7958,23 +10719,65 @@
       <c r="S5" s="5">
         <v>19.984000000000002</v>
       </c>
-      <c r="U5" s="17" t="s">
+      <c r="U5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="V5" s="18">
+      <c r="V5" s="17">
         <v>16.884</v>
       </c>
-      <c r="W5" s="18">
+      <c r="W5" s="17">
         <v>7.427999999999999</v>
       </c>
-      <c r="X5" s="18">
+      <c r="X5" s="17">
         <v>2.4349999999999996</v>
       </c>
-      <c r="Y5" s="19">
+      <c r="Y5" s="18">
         <v>1.3259999999999996</v>
       </c>
+      <c r="AD5" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE5" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF5" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG5" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI5" s="25">
+        <v>43.7</v>
+      </c>
+      <c r="AJ5" s="25">
+        <v>13.4</v>
+      </c>
+      <c r="AK5" s="25">
+        <v>3.45</v>
+      </c>
+      <c r="AL5" s="26">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="AN5" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO5" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV5">
+        <v>60</v>
+      </c>
+      <c r="AW5">
+        <v>43.3</v>
+      </c>
+      <c r="AX5">
+        <v>72.2</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" ht="60" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:50" ht="60" x14ac:dyDescent="0.45">
       <c r="I6" s="9" t="s">
         <v>23</v>
       </c>
@@ -8005,13 +10808,85 @@
       <c r="S6" s="5">
         <v>3.69</v>
       </c>
+      <c r="AD6" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE6" s="22">
+        <v>27.87</v>
+      </c>
+      <c r="AF6" s="22">
+        <v>25.06</v>
+      </c>
+      <c r="AG6" s="22">
+        <v>31.97</v>
+      </c>
+      <c r="AI6" s="25">
+        <v>60.584000000000003</v>
+      </c>
+      <c r="AJ6" s="25">
+        <v>20.827999999999999</v>
+      </c>
+      <c r="AK6" s="25">
+        <v>5.8849999999999998</v>
+      </c>
+      <c r="AL6" s="26">
+        <v>5.476</v>
+      </c>
+      <c r="AN6" s="22">
+        <v>27.87</v>
+      </c>
+      <c r="AO6" s="22">
+        <v>17.2</v>
+      </c>
+      <c r="AP6" s="22"/>
+      <c r="AQ6" s="22"/>
+      <c r="AR6" s="22"/>
+      <c r="AV6">
+        <v>86.7</v>
+      </c>
+      <c r="AW6">
+        <v>43.3</v>
+      </c>
+      <c r="AX6">
+        <v>72.2</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:50" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
+      <c r="AD7" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE7" s="22">
+        <v>17.2</v>
+      </c>
+      <c r="AF7" s="22">
+        <v>16.8</v>
+      </c>
+      <c r="AG7" s="22">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="AN7" s="22">
+        <v>25.06</v>
+      </c>
+      <c r="AO7" s="22">
+        <v>16.8</v>
+      </c>
+      <c r="AP7" s="22"/>
+      <c r="AQ7" s="22"/>
+      <c r="AR7" s="22"/>
+      <c r="AV7">
+        <v>86.7</v>
+      </c>
+      <c r="AW7">
+        <v>65</v>
+      </c>
+      <c r="AX7">
+        <v>72.2</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:50" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -8030,8 +10905,27 @@
       <c r="M8" s="8" t="s">
         <v>19</v>
       </c>
+      <c r="AD8" s="23"/>
+      <c r="AN8" s="22">
+        <v>31.97</v>
+      </c>
+      <c r="AO8" s="22">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="AP8" s="22"/>
+      <c r="AQ8" s="22"/>
+      <c r="AR8" s="22"/>
+      <c r="AV8">
+        <v>72.2</v>
+      </c>
+      <c r="AW8">
+        <v>65</v>
+      </c>
+      <c r="AX8">
+        <v>130</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:50" ht="15" x14ac:dyDescent="0.45">
       <c r="I9" s="3" t="s">
         <v>20</v>
       </c>
@@ -8047,8 +10941,26 @@
       <c r="M9" s="5">
         <v>19.984000000000002</v>
       </c>
+      <c r="AN9" s="25">
+        <v>60.584000000000003</v>
+      </c>
+      <c r="AO9" s="25">
+        <v>43.7</v>
+      </c>
+      <c r="AP9" s="22"/>
+      <c r="AQ9" s="22"/>
+      <c r="AR9" s="22"/>
+      <c r="AV9">
+        <v>72.2</v>
+      </c>
+      <c r="AW9">
+        <v>65</v>
+      </c>
+      <c r="AX9">
+        <v>130</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:50" ht="15" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -8067,28 +10979,60 @@
       <c r="M10" s="5">
         <v>5.476</v>
       </c>
+      <c r="AN10" s="25">
+        <v>20.827999999999999</v>
+      </c>
+      <c r="AO10" s="25">
+        <v>13.4</v>
+      </c>
+      <c r="AV10">
+        <v>60</v>
+      </c>
+      <c r="AW10">
+        <v>72.2</v>
+      </c>
+      <c r="AX10">
+        <v>86.7</v>
+      </c>
     </row>
-    <row r="11" spans="1:25" ht="30" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:50" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="13" t="s">
+      <c r="O11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="P11" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="Q11" s="14" t="s">
+      <c r="Q11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="R11" s="14" t="s">
+      <c r="R11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="S11" s="15" t="s">
+      <c r="S11" s="14" t="s">
         <v>19</v>
       </c>
+      <c r="AD11" s="23"/>
+      <c r="AE11" s="24"/>
+      <c r="AN11" s="25">
+        <v>5.8849999999999998</v>
+      </c>
+      <c r="AO11" s="25">
+        <v>3.45</v>
+      </c>
+      <c r="AV11">
+        <v>72.2</v>
+      </c>
+      <c r="AW11">
+        <v>58.5</v>
+      </c>
+      <c r="AX11">
+        <v>86.7</v>
+      </c>
     </row>
-    <row r="12" spans="1:25" ht="60" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:50" ht="60" x14ac:dyDescent="0.45">
       <c r="O12" s="3" t="s">
         <v>23</v>
       </c>
@@ -8104,8 +11048,23 @@
       <c r="S12" s="5">
         <v>4.1500000000000004</v>
       </c>
+      <c r="AN12" s="26">
+        <v>5.476</v>
+      </c>
+      <c r="AO12" s="26">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="AV12">
+        <v>72.2</v>
+      </c>
+      <c r="AW12">
+        <v>65</v>
+      </c>
+      <c r="AX12">
+        <v>86.7</v>
+      </c>
     </row>
-    <row r="13" spans="1:25" ht="30" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:50" ht="30" x14ac:dyDescent="0.45">
       <c r="O13" s="3" t="s">
         <v>26</v>
       </c>
@@ -8121,28 +11080,70 @@
       <c r="S13" s="5">
         <v>5.476</v>
       </c>
+      <c r="AD13" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE13" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF13" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG13" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AV13">
+        <v>72.2</v>
+      </c>
+      <c r="AW13">
+        <v>115.6</v>
+      </c>
+      <c r="AX13">
+        <v>115.6</v>
+      </c>
     </row>
-    <row r="14" spans="1:25" ht="15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:50" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="O14" s="16" t="s">
+      <c r="O14" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="P14" s="12">
+      <c r="P14" s="2">
         <v>16.884</v>
       </c>
-      <c r="Q14" s="12">
+      <c r="Q14" s="2">
         <v>7.427999999999999</v>
       </c>
-      <c r="R14" s="12">
+      <c r="R14" s="2">
         <v>2.4349999999999996</v>
       </c>
-      <c r="S14" s="12">
+      <c r="S14" s="2">
         <v>1.3259999999999996</v>
       </c>
+      <c r="AD14" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE14" s="22">
+        <v>27.87</v>
+      </c>
+      <c r="AF14" s="22">
+        <v>25.06</v>
+      </c>
+      <c r="AG14" s="22">
+        <v>31.97</v>
+      </c>
+      <c r="AV14">
+        <v>72.2</v>
+      </c>
+      <c r="AW14">
+        <v>57.8</v>
+      </c>
+      <c r="AX14">
+        <v>115.6</v>
+      </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:50" ht="28.5" x14ac:dyDescent="0.45">
       <c r="O15" t="s">
         <v>27</v>
       </c>
@@ -8162,49 +11163,188 @@
         <f t="shared" si="0"/>
         <v>31.952000000000002</v>
       </c>
+      <c r="AD15" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE15" s="22">
+        <f xml:space="preserve"> 0.7283*AE14- 0.7162</f>
+        <v>19.581520999999999</v>
+      </c>
+      <c r="AF15" s="22">
+        <f t="shared" ref="AF15" si="1" xml:space="preserve"> 0.7283*AF14- 0.7162</f>
+        <v>17.534997999999998</v>
+      </c>
+      <c r="AG15" s="22">
+        <f xml:space="preserve"> 0.7283*AG14- 0.7162</f>
+        <v>22.567550999999998</v>
+      </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:50" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>9</v>
       </c>
+      <c r="AD16" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE16" s="22">
+        <v>17.2</v>
+      </c>
+      <c r="AF16" s="22">
+        <v>16.8</v>
+      </c>
+      <c r="AG16" s="22">
+        <v>32.700000000000003</v>
+      </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.45">
+      <c r="AD17" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE17">
+        <f>ABS((AE16-AE15)/AE16) * 100</f>
+        <v>13.846052325581393</v>
+      </c>
+      <c r="AF17">
+        <f>ABS((AF16-AF15)/AF16) * 100</f>
+        <v>4.3749880952380797</v>
+      </c>
+      <c r="AG17">
+        <f>ABS((AG16-AG15)/AG16) * 100</f>
+        <v>30.986082568807348</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" ht="57" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>10</v>
       </c>
+      <c r="AD18" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE18" s="24">
+        <f>AVERAGE(AE17:AG17)/100</f>
+        <v>0.1640237432987561</v>
+      </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="2">
+  <tableParts count="5">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>